<commit_message>
renamed medication valuesets so they are ordered in the artificacts table
</commit_message>
<xml_diff>
--- a/docs/ValueSet-med-alemtuzumab-vs.xlsx
+++ b/docs/ValueSet-med-alemtuzumab-vs.xlsx
@@ -36,7 +36,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Alemtuzumab</t>
+    <t>RxNormAlemtuzumabVS</t>
   </si>
   <si>
     <t>Title</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-07-29T15:34:16-05:00</t>
+    <t>2022-07-29T16:31:05-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>